<commit_message>
Updating testcases of converting
</commit_message>
<xml_diff>
--- a/Documents/Test cases/Version 1/Test Cases and bug report V1.xlsx
+++ b/Documents/Test cases/Version 1/Test Cases and bug report V1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HET SEM-1\CPR 101\Final project\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vansh\Documents\GitHub\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEECCC5-AF41-4AFA-A44B-9B5ABF488785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2871AB4-7756-4C99-B6B8-F8DD9CF80DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="converting" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Test case No.</t>
   </si>
@@ -52,6 +52,84 @@
   </si>
   <si>
     <t>Tester name:  HET PANKITKUMAR PARIKH</t>
+  </si>
+  <si>
+    <t>This should give all the integer in the input entered</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Program end</t>
+  </si>
+  <si>
+    <t>Programs Ends</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Case 8</t>
+  </si>
+  <si>
+    <t>It Should extract the Integer from the input entered</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>@122eee'</t>
+  </si>
+  <si>
+    <t>Case 7</t>
+  </si>
+  <si>
+    <t>+12@'</t>
+  </si>
+  <si>
+    <t>Case 6</t>
+  </si>
+  <si>
+    <t>To see if any special case are entered will it give any output</t>
+  </si>
+  <si>
+    <t>manav@1246</t>
+  </si>
+  <si>
+    <t>Case 5</t>
+  </si>
+  <si>
+    <t>If no string is entered then it should give 0 as output</t>
+  </si>
+  <si>
+    <t>" "</t>
+  </si>
+  <si>
+    <t>Case 4</t>
+  </si>
+  <si>
+    <t>123g32</t>
+  </si>
+  <si>
+    <t>Case 3</t>
+  </si>
+  <si>
+    <t>it should give 0 a there is no int in the input entered</t>
+  </si>
+  <si>
+    <t>fgd</t>
+  </si>
+  <si>
+    <t>Case 2</t>
+  </si>
+  <si>
+    <t>123gg</t>
+  </si>
+  <si>
+    <t>Case 1</t>
+  </si>
+  <si>
+    <t>Tester name:  Manav Dineshbhai Dhameliya</t>
   </si>
 </sst>
 </file>
@@ -87,9 +165,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,21 +452,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="20.7265625" customWidth="1"/>
-    <col min="6" max="6" width="85.7265625" customWidth="1"/>
+    <col min="1" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="85.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -392,7 +474,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -410,6 +492,166 @@
       </c>
       <c r="F2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>123</v>
+      </c>
+      <c r="D3">
+        <v>123</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>123</v>
+      </c>
+      <c r="D5">
+        <v>12332</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1246</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>122</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -428,13 +670,13 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="20.7265625" customWidth="1"/>
-    <col min="6" max="6" width="85.7265625" customWidth="1"/>
+    <col min="1" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="85.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -444,7 +686,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -476,17 +718,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D3B1AA-0F13-4019-BF13-01FFE44DE918}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="20.7265625" customWidth="1"/>
-    <col min="6" max="6" width="85.7265625" customWidth="1"/>
+    <col min="1" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="85.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -496,7 +738,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -532,13 +774,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="20.7265625" customWidth="1"/>
-    <col min="6" max="6" width="85.7265625" customWidth="1"/>
+    <col min="1" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="85.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -548,7 +790,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Uploading source code, test case output of Manipulating module and updating test case excel file
</commit_message>
<xml_diff>
--- a/Documents/Test cases/Version 1/Test Cases and bug report V1.xlsx
+++ b/Documents/Test cases/Version 1/Test Cases and bug report V1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vansh\Documents\GitHub\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HET SEM-1\CPR 101\Final project\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2871AB4-7756-4C99-B6B8-F8DD9CF80DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E5AB40-9CF0-41C2-902B-3EFF3F7FE603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="converting" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>Test case No.</t>
   </si>
@@ -130,6 +130,69 @@
   </si>
   <si>
     <t>Tester name:  Manav Dineshbhai Dhameliya</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>The function is working as expected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                ######</t>
+  </si>
+  <si>
+    <t>######$$$$$$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               $$$$$$</t>
+  </si>
+  <si>
+    <t>My name is Het Parikh</t>
+  </si>
+  <si>
+    <t>qwertyuiopasdfghjklzxcvbnmqwertyuiopasdfghjklzxcvbnmqwertyuiopasdfghjklzxcvbnm</t>
+  </si>
+  <si>
+    <t>qwertyuiopasdfghjklzxcvbnmqwertyuiopasdfghjklzxcvbnmqwertyuiopasdfghjklzxcvbnmqwertyuiopasdfghjklzxcvbnmqwertyuiopasdfghjklzxcvbnmqwertyuiopasdfghjklzxcvbnm</t>
+  </si>
+  <si>
+    <t>The program should  give an error as MAX BUFFER SIZE IS 80.</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>The function should  give an error as MAX BUFFER SIZE IS 80, but it didn't cause any error.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>It should give an error on the screen, if a newline is entered as input</t>
+  </si>
+  <si>
+    <t>Recommended fix: there should be condition which checks length of first string and if it exceeds 79 characters, it should give an error to enter it again.</t>
+  </si>
+  <si>
+    <t>It exit the application by printing the closing statement</t>
+  </si>
+  <si>
+    <t>Should exit the application by printing the closing statement</t>
+  </si>
+  <si>
+    <t>The program quits as expected</t>
+  </si>
+  <si>
+    <t>1234567891011</t>
+  </si>
+  <si>
+    <t>My name is</t>
+  </si>
+  <si>
+    <t>Het Parikh</t>
   </si>
 </sst>
 </file>
@@ -165,13 +228,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,27 +529,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="20.77734375" customWidth="1"/>
-    <col min="6" max="6" width="85.77734375" customWidth="1"/>
+    <col min="1" max="5" width="20.81640625" customWidth="1"/>
+    <col min="6" max="6" width="85.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -494,7 +569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -507,14 +582,14 @@
       <c r="D3">
         <v>123</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -527,14 +602,14 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -547,14 +622,14 @@
       <c r="D5">
         <v>12332</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -567,14 +642,14 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -587,18 +662,18 @@
       <c r="D7">
         <v>1246</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C8">
@@ -607,18 +682,18 @@
       <c r="D8">
         <v>12</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C9">
@@ -627,14 +702,14 @@
       <c r="D9">
         <v>122</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -647,7 +722,7 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
@@ -670,23 +745,23 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="20.77734375" customWidth="1"/>
-    <col min="6" max="6" width="85.77734375" customWidth="1"/>
+    <col min="1" max="5" width="20.81640625" customWidth="1"/>
+    <col min="6" max="6" width="85.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -716,29 +791,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D3B1AA-0F13-4019-BF13-01FFE44DE918}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="20.77734375" customWidth="1"/>
-    <col min="6" max="6" width="85.77734375" customWidth="1"/>
+    <col min="1" max="5" width="20.81640625" customWidth="1"/>
+    <col min="6" max="6" width="85.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -758,9 +833,194 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>123456</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="4">
+        <v>7891011</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="116" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="5"/>
+      <c r="B10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="5"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="8">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C9:C10"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -774,23 +1034,23 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="20.77734375" customWidth="1"/>
-    <col min="6" max="6" width="85.77734375" customWidth="1"/>
+    <col min="1" max="5" width="20.81640625" customWidth="1"/>
+    <col min="6" max="6" width="85.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Update to test case excel file
</commit_message>
<xml_diff>
--- a/Documents/Test cases/Version 1/Test Cases and bug report V1.xlsx
+++ b/Documents/Test cases/Version 1/Test Cases and bug report V1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HET SEM-1\CPR 101\Final project\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6d68bcfb44c4b5b/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E5AB40-9CF0-41C2-902B-3EFF3F7FE603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1B0CEC-05AF-4223-9B64-40B5D0576407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="converting" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="66">
   <si>
     <t>Test case No.</t>
   </si>
@@ -193,6 +193,39 @@
   </si>
   <si>
     <t>Het Parikh</t>
+  </si>
+  <si>
+    <t>Manav</t>
+  </si>
+  <si>
+    <t>Seneca</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Markham</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -234,15 +267,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -533,23 +566,23 @@
       <selection sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="20.81640625" customWidth="1"/>
-    <col min="6" max="6" width="85.81640625" customWidth="1"/>
+    <col min="1" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="85.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -569,7 +602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -589,7 +622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -609,7 +642,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -629,7 +662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -649,7 +682,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -669,7 +702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -689,7 +722,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -709,7 +742,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -739,29 +772,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440B6FB4-A523-4D5A-9DD8-CBB4B7170EE4}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="20.81640625" customWidth="1"/>
-    <col min="6" max="6" width="85.81640625" customWidth="1"/>
+    <col min="1" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="85.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -779,6 +812,126 @@
       </c>
       <c r="F2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -793,27 +946,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D3B1AA-0F13-4019-BF13-01FFE44DE918}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="20.81640625" customWidth="1"/>
-    <col min="6" max="6" width="85.81640625" customWidth="1"/>
+    <col min="1" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="85.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -833,183 +986,183 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>123456</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="3">
         <v>7891011</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="116" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="115.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
         <v>4</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
         <v>5</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
         <v>6</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1034,23 +1187,23 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="20.81640625" customWidth="1"/>
-    <col min="6" max="6" width="85.81640625" customWidth="1"/>
+    <col min="1" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="85.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>

</xml_diff>